<commit_message>
Sprint 2: Added Sprint 2 Backlog as new sheet to Sprint Backlog - Tasks-1.xlsx
</commit_message>
<xml_diff>
--- a/Sprint Backlog - Tasks-1.xlsx
+++ b/Sprint Backlog - Tasks-1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhichappidi/PycharmProjects/SoftwareEngineeringProject/FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68B31045-ABB1-1B43-B81A-25EB779885F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9126D27-1808-3548-8F8A-82180BA764B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="4760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="18580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
@@ -174,13 +175,73 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>User Story #6 -Order Management (13 SP)</t>
+  </si>
+  <si>
+    <t>User Story #7 - Update Customer Information (5 SP)</t>
+  </si>
+  <si>
+    <t>User Story #8 - Delete Review (3 SP)</t>
+  </si>
+  <si>
+    <t>User Story #9 - Update Ingredient (5 SP)</t>
+  </si>
+  <si>
+    <t>User Story #10 - Search Sandwich by ID (4 SP)</t>
+  </si>
+  <si>
+    <t>Implement GET /sandwiches/{id}</t>
+  </si>
+  <si>
+    <t>Unit test for sandwich retrieval by ID</t>
+  </si>
+  <si>
+    <t>Implement PUT /ingredients/{id}</t>
+  </si>
+  <si>
+    <t>Unit test for updating ingredient</t>
+  </si>
+  <si>
+    <t>Implement DELETE /reviews/{id}</t>
+  </si>
+  <si>
+    <t>Unit test for deleting review</t>
+  </si>
+  <si>
+    <t>Implement PUT /customers/{id}</t>
+  </si>
+  <si>
+    <t>Add schema for customer update</t>
+  </si>
+  <si>
+    <t>Unit test for customer update</t>
+  </si>
+  <si>
+    <t>Create Order model/schema</t>
+  </si>
+  <si>
+    <t>Implement POST /orders endpoint</t>
+  </si>
+  <si>
+    <t>Implement GET /orders endpoint</t>
+  </si>
+  <si>
+    <t>Implement GET /orders/{id}</t>
+  </si>
+  <si>
+    <t>Wire up order router + load_routes()</t>
+  </si>
+  <si>
+    <t>Unit test for orders (test_orders)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -221,6 +282,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;⋎ntury Gothic\&quot;&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -334,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,6 +438,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,8 +659,8 @@
   </sheetPr>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1725,4 +1794,918 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD405797-6405-3348-9E90-A306D1608359}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" ht="13">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="4">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:J4" si="0">SUM(D5:D10)</f>
+        <v>9</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="13">
+      <c r="A5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="13">
+      <c r="A6" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13">
+      <c r="A7" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13">
+      <c r="A8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="13">
+      <c r="A9" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="13">
+      <c r="A10" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="4">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5">
+        <f>SUM(D12:D14)</f>
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <f>SUM(E12:E14)</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="5">
+        <f>SUM(F12:F14)</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <f>SUM(G12:G14)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <f>SUM(H12:H14)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f>SUM(I12:I14)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <f>SUM(J12:J14)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="13">
+      <c r="A12" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="13">
+      <c r="A13" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="13">
+      <c r="A14" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5">
+        <f>SUM(D16:D17)</f>
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="5">
+        <f>SUM(E16:E17)</f>
+        <v>0.75</v>
+      </c>
+      <c r="F15" s="5">
+        <f>SUM(F16:F17)</f>
+        <v>0.75</v>
+      </c>
+      <c r="G15" s="5">
+        <f>SUM(G16:G17)</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <f>SUM(H16:H17)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <f>SUM(I16:I17)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <f>SUM(J16:J17)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="13">
+      <c r="A16" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13">
+      <c r="A17" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="4">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5">
+        <f>SUM(D19:D20)</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="5">
+        <f>SUM(E19:E20)</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <f>SUM(F19:F20)</f>
+        <v>2</v>
+      </c>
+      <c r="G18" s="5">
+        <f>SUM(G19:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <f>SUM(H19:H20)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <f>SUM(I19:I20)</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <f>SUM(J19:J20)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" ht="13">
+      <c r="A19" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="8">
+        <v>3</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="10">
+        <v>2</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13">
+      <c r="A20" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="4">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5">
+        <f>SUM(D22:D23)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="5">
+        <f>SUM(E22:E23)</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <f>SUM(F22:F23)</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <f>SUM(G22:G23)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="5">
+        <f>SUM(H22:H23)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <f>SUM(I22:I23)</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <f>SUM(J22:J23)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" ht="13">
+      <c r="A22" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="8">
+        <v>3</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+      <c r="I22" s="10">
+        <v>0</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13">
+      <c r="A23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0</v>
+      </c>
+      <c r="J23" s="10">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13">
+      <c r="A24" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13">
+        <f>D4+D11+D15+D18+D21</f>
+        <v>19</v>
+      </c>
+      <c r="E24" s="13">
+        <f>E4+E11+E15+E18+E21</f>
+        <v>6.75</v>
+      </c>
+      <c r="F24" s="13">
+        <f>F4+F11+F15+F18+F21</f>
+        <v>6.75</v>
+      </c>
+      <c r="G24" s="13">
+        <f>G4+G11+G15+G18+G21</f>
+        <v>3.5</v>
+      </c>
+      <c r="H24" s="13">
+        <f>H4+H11+H15+H18+H21</f>
+        <v>1.5</v>
+      </c>
+      <c r="I24" s="13">
+        <f>I4+I11+I15+I18+I21</f>
+        <v>1</v>
+      </c>
+      <c r="J24" s="13">
+        <f>J4+J11+J15+J18+J21</f>
+        <v>0.5</v>
+      </c>
+      <c r="K24" s="12"/>
+      <c r="L24" s="13">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:K23" xr:uid="{92A62C36-DEEE-B24D-9F03-BEF2846C19E5}">
+      <formula1>"To Do,Doing,Done"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Project: Integrated full MySQL support, fixed model/routing issues, implemented ingredient depletion and promo code logic, ensured full API functionality
</commit_message>
<xml_diff>
--- a/Sprint Backlog - Tasks-1.xlsx
+++ b/Sprint Backlog - Tasks-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhichappidi/PycharmProjects/SoftwareEngineeringProject/FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9126D27-1808-3548-8F8A-82180BA764B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8C4A04-D370-8C4D-AFBB-393642B65C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="18580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4480" yWindow="920" windowWidth="25600" windowHeight="18580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Unit test for orders (test_orders)</t>
+  </si>
+  <si>
+    <t>User Story #11 - Search Sandwich by ID (4 SP)</t>
   </si>
 </sst>
 </file>
@@ -429,6 +432,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,7 +442,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,36 +674,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="18"/>
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:12" ht="13">
       <c r="A3" s="1" t="s">
@@ -1801,10 +1804,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1815,36 +1818,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="18"/>
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:12" ht="13">
       <c r="A3" s="1" t="s">
@@ -1926,7 +1929,7 @@
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="13">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B5" s="8">
@@ -1964,7 +1967,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="13">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="8">
@@ -2002,7 +2005,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="13">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>63</v>
       </c>
       <c r="B7" s="8">
@@ -2040,7 +2043,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="13">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>64</v>
       </c>
       <c r="B8" s="8">
@@ -2078,7 +2081,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="13">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B9" s="8">
@@ -2114,7 +2117,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="13">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="8">
@@ -2160,31 +2163,31 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5">
-        <f>SUM(D12:D14)</f>
+        <f t="shared" ref="D11:J11" si="1">SUM(D12:D14)</f>
         <v>3</v>
       </c>
       <c r="E11" s="5">
-        <f>SUM(E12:E14)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F11" s="5">
-        <f>SUM(F12:F14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G11" s="5">
-        <f>SUM(G12:G14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H11" s="5">
-        <f>SUM(H12:H14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I11" s="5">
-        <f>SUM(I12:I14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J11" s="5">
-        <f>SUM(J12:J14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -2193,7 +2196,7 @@
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="13">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="8">
@@ -2231,7 +2234,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="13">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="8">
@@ -2269,7 +2272,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="13">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="8">
@@ -2315,31 +2318,31 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5">
-        <f>SUM(D16:D17)</f>
+        <f t="shared" ref="D15:J15" si="2">SUM(D16:D17)</f>
         <v>1.5</v>
       </c>
       <c r="E15" s="5">
-        <f>SUM(E16:E17)</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="F15" s="5">
-        <f>SUM(F16:F17)</f>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="G15" s="5">
-        <f>SUM(G16:G17)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H15" s="5">
-        <f>SUM(H16:H17)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I15" s="5">
-        <f>SUM(I16:I17)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J15" s="5">
-        <f>SUM(J16:J17)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K15" s="6" t="s">
@@ -2348,7 +2351,7 @@
       <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" ht="13">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="8">
@@ -2386,7 +2389,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="13">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="8">
@@ -2432,31 +2435,31 @@
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5">
-        <f>SUM(D19:D20)</f>
+        <f t="shared" ref="D18:J18" si="3">SUM(D19:D20)</f>
         <v>3</v>
       </c>
       <c r="E18" s="5">
-        <f>SUM(E19:E20)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F18" s="5">
-        <f>SUM(F19:F20)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G18" s="5">
-        <f>SUM(G19:G20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H18" s="5">
-        <f>SUM(H19:H20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I18" s="5">
-        <f>SUM(I19:I20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J18" s="5">
-        <f>SUM(J19:J20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K18" s="6" t="s">
@@ -2465,7 +2468,7 @@
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="13">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="8">
@@ -2503,7 +2506,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="13">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="8">
@@ -2582,7 +2585,7 @@
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" ht="13">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="14" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="8">
@@ -2657,42 +2660,159 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="13">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:12" ht="16">
+      <c r="A24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="4">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5">
+        <f>SUM(D25:D26)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E24" s="5">
+        <f>SUM(E25:E26)</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="5">
+        <f>SUM(F25:F26)</f>
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <f>SUM(G25:G26)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H24" s="5">
+        <f>SUM(H25:H26)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <f>SUM(I25:I26)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <f>SUM(J25:J26)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="8">
+        <v>3</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+      <c r="I25" s="10">
+        <v>0</v>
+      </c>
+      <c r="J25" s="10">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10">
+        <v>0</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A27" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="13">
         <f>D4+D11+D15+D18+D21</f>
         <v>19</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E27" s="13">
         <f>E4+E11+E15+E18+E21</f>
         <v>6.75</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F27" s="13">
         <f>F4+F11+F15+F18+F21</f>
         <v>6.75</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G27" s="13">
         <f>G4+G11+G15+G18+G21</f>
         <v>3.5</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H27" s="13">
         <f>H4+H11+H15+H18+H21</f>
         <v>1.5</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I27" s="13">
         <f>I4+I11+I15+I18+I21</f>
         <v>1</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J27" s="13">
         <f>J4+J11+J15+J18+J21</f>
         <v>0.5</v>
       </c>
-      <c r="K24" s="12"/>
-      <c r="L24" s="13">
+      <c r="K27" s="12"/>
+      <c r="L27" s="13">
         <v>14</v>
       </c>
     </row>
@@ -2702,7 +2822,7 @@
     <mergeCell ref="A2:L2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:K23" xr:uid="{92A62C36-DEEE-B24D-9F03-BEF2846C19E5}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:K26" xr:uid="{92A62C36-DEEE-B24D-9F03-BEF2846C19E5}">
       <formula1>"To Do,Doing,Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>